<commit_message>
week 3 files of Excel
</commit_message>
<xml_diff>
--- a/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 3/W3_V1 IntroNamedRanges.xlsx
+++ b/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 3/W3_V1 IntroNamedRanges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\Excel Skills for Business Intermediate I\Week 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2418AB67-EC21-43E2-8FA8-66C5F09203BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6943B6F9-3CB1-4AF6-8BC0-43DD32CD37D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,22 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$4:$H$24</definedName>
+    <definedName name="Annual_Salary">Staff!$N$4:$N$38</definedName>
+    <definedName name="Date_of_Hire">Staff!$F$4:$F$38</definedName>
+    <definedName name="Department">Staff!$H$4:$H$38</definedName>
+    <definedName name="Email">Staff!$E$4:$E$38</definedName>
+    <definedName name="emp_ID">Staff!$A$4:$A$38</definedName>
+    <definedName name="Extension">Staff!$K$4:$K$38</definedName>
+    <definedName name="First">Staff!$C$4:$C$38</definedName>
+    <definedName name="Floor">Staff!$J$4:$J$38</definedName>
+    <definedName name="Gender">Staff!$D$4:$D$38</definedName>
+    <definedName name="Last">Staff!$B$4:$B$38</definedName>
+    <definedName name="Last_Review">Staff!$L$4:$L$38</definedName>
+    <definedName name="Location">Staff!$I$4:$I$38</definedName>
+    <definedName name="Next_Review">Staff!$M$4:$M$38</definedName>
+    <definedName name="Pension">Staff!$O$4:$O$38</definedName>
     <definedName name="pension_rate">Staff!$P$1</definedName>
+    <definedName name="Years_Service">Staff!$G$4:$G$38</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1031,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4:N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,7 +1148,7 @@
       </c>
       <c r="G4" s="5">
         <f t="shared" ref="G4:G38" ca="1" si="1">YEARFRAC(F4,TODAY())</f>
-        <v>19.683333333333334</v>
+        <v>19.68611111111111</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>33</v>
@@ -1160,7 +1175,7 @@
         <v>101400</v>
       </c>
       <c r="O4" s="15">
-        <f xml:space="preserve"> N4*pension_rate</f>
+        <f t="shared" ref="O4:O38" si="5" xml:space="preserve"> N4*pension_rate</f>
         <v>9126</v>
       </c>
     </row>
@@ -1186,7 +1201,7 @@
       </c>
       <c r="G5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>19.611111111111111</v>
+        <v>19.613888888888887</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>80</v>
@@ -1213,7 +1228,7 @@
         <v>70300</v>
       </c>
       <c r="O5" s="15">
-        <f xml:space="preserve"> N5*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>6327</v>
       </c>
     </row>
@@ -1239,7 +1254,7 @@
       </c>
       <c r="G6" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>18.072222222222223</v>
+        <v>18.074999999999999</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>72</v>
@@ -1266,7 +1281,7 @@
         <v>68800</v>
       </c>
       <c r="O6" s="15">
-        <f xml:space="preserve"> N6*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>6192</v>
       </c>
     </row>
@@ -1292,7 +1307,7 @@
       </c>
       <c r="G7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>16.458333333333332</v>
+        <v>16.461111111111112</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>35</v>
@@ -1319,7 +1334,7 @@
         <v>59200</v>
       </c>
       <c r="O7" s="15">
-        <f xml:space="preserve"> N7*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5328</v>
       </c>
     </row>
@@ -1345,7 +1360,7 @@
       </c>
       <c r="G8" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>15.227777777777778</v>
+        <v>15.230555555555556</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>72</v>
@@ -1372,7 +1387,7 @@
         <v>62900</v>
       </c>
       <c r="O8" s="15">
-        <f xml:space="preserve"> N8*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5661</v>
       </c>
     </row>
@@ -1398,7 +1413,7 @@
       </c>
       <c r="G9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>14.694444444444445</v>
+        <v>14.697222222222223</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>35</v>
@@ -1425,7 +1440,7 @@
         <v>58400</v>
       </c>
       <c r="O9" s="15">
-        <f xml:space="preserve"> N9*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5256</v>
       </c>
     </row>
@@ -1451,7 +1466,7 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>14.541666666666666</v>
+        <v>14.544444444444444</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>72</v>
@@ -1478,7 +1493,7 @@
         <v>59200</v>
       </c>
       <c r="O10" s="15">
-        <f xml:space="preserve"> N10*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5328</v>
       </c>
     </row>
@@ -1504,7 +1519,7 @@
       </c>
       <c r="G11" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>13.930555555555555</v>
+        <v>13.933333333333334</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>20</v>
@@ -1531,7 +1546,7 @@
         <v>51600</v>
       </c>
       <c r="O11" s="15">
-        <f xml:space="preserve"> N11*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4644</v>
       </c>
     </row>
@@ -1557,7 +1572,7 @@
       </c>
       <c r="G12" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>12.483333333333333</v>
+        <v>12.486111111111111</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>72</v>
@@ -1584,7 +1599,7 @@
         <v>58200</v>
       </c>
       <c r="O12" s="15">
-        <f xml:space="preserve"> N12*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5238</v>
       </c>
     </row>
@@ -1610,7 +1625,7 @@
       </c>
       <c r="G13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>12.113888888888889</v>
+        <v>12.116666666666667</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
@@ -1637,7 +1652,7 @@
         <v>55800</v>
       </c>
       <c r="O13" s="15">
-        <f xml:space="preserve"> N13*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5022</v>
       </c>
     </row>
@@ -1663,7 +1678,7 @@
       </c>
       <c r="G14" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>10.816666666666666</v>
+        <v>10.819444444444445</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>72</v>
@@ -1690,7 +1705,7 @@
         <v>55500</v>
       </c>
       <c r="O14" s="15">
-        <f xml:space="preserve"> N14*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4995</v>
       </c>
     </row>
@@ -1716,7 +1731,7 @@
       </c>
       <c r="G15" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>10.655555555555555</v>
+        <v>10.658333333333333</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>80</v>
@@ -1743,7 +1758,7 @@
         <v>48400</v>
       </c>
       <c r="O15" s="15">
-        <f xml:space="preserve"> N15*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4356</v>
       </c>
     </row>
@@ -1769,7 +1784,7 @@
       </c>
       <c r="G16" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6277777777777782</v>
+        <v>9.6305555555555564</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>72</v>
@@ -1796,7 +1811,7 @@
         <v>59300</v>
       </c>
       <c r="O16" s="15">
-        <f xml:space="preserve"> N16*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5337</v>
       </c>
     </row>
@@ -1822,7 +1837,7 @@
       </c>
       <c r="G17" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3000000000000007</v>
+        <v>9.3027777777777771</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>72</v>
@@ -1849,7 +1864,7 @@
         <v>56000</v>
       </c>
       <c r="O17" s="15">
-        <f xml:space="preserve"> N17*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5040</v>
       </c>
     </row>
@@ -1875,7 +1890,7 @@
       </c>
       <c r="G18" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>8.530555555555555</v>
+        <v>8.5333333333333332</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>22</v>
@@ -1902,7 +1917,7 @@
         <v>63200</v>
       </c>
       <c r="O18" s="15">
-        <f xml:space="preserve"> N18*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5688</v>
       </c>
     </row>
@@ -1928,7 +1943,7 @@
       </c>
       <c r="G19" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0388888888888896</v>
+        <v>8.0416666666666661</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
@@ -1955,7 +1970,7 @@
         <v>51700</v>
       </c>
       <c r="O19" s="15">
-        <f xml:space="preserve"> N19*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4653</v>
       </c>
     </row>
@@ -1981,7 +1996,7 @@
       </c>
       <c r="G20" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9416666666666664</v>
+        <v>7.9444444444444446</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>80</v>
@@ -2008,7 +2023,7 @@
         <v>49600</v>
       </c>
       <c r="O20" s="15">
-        <f xml:space="preserve"> N20*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4464</v>
       </c>
     </row>
@@ -2034,7 +2049,7 @@
       </c>
       <c r="G21" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>7.416666666666667</v>
+        <v>7.4194444444444443</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>35</v>
@@ -2061,7 +2076,7 @@
         <v>45100</v>
       </c>
       <c r="O21" s="15">
-        <f xml:space="preserve"> N21*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4059</v>
       </c>
     </row>
@@ -2087,7 +2102,7 @@
       </c>
       <c r="G22" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3583333333333334</v>
+        <v>6.3611111111111107</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
@@ -2114,7 +2129,7 @@
         <v>42100</v>
       </c>
       <c r="O22" s="15">
-        <f xml:space="preserve"> N22*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>3789</v>
       </c>
     </row>
@@ -2140,7 +2155,7 @@
       </c>
       <c r="G23" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>6.072222222222222</v>
+        <v>6.0750000000000002</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>20</v>
@@ -2167,7 +2182,7 @@
         <v>62800</v>
       </c>
       <c r="O23" s="15">
-        <f xml:space="preserve"> N23*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5652</v>
       </c>
     </row>
@@ -2193,7 +2208,7 @@
       </c>
       <c r="G24" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0444444444444443</v>
+        <v>6.0472222222222225</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>72</v>
@@ -2220,7 +2235,7 @@
         <v>54700</v>
       </c>
       <c r="O24" s="15">
-        <f xml:space="preserve"> N24*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4923</v>
       </c>
     </row>
@@ -2246,7 +2261,7 @@
       </c>
       <c r="G25" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9</v>
+        <v>5.9027777777777777</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>72</v>
@@ -2273,7 +2288,7 @@
         <v>52600</v>
       </c>
       <c r="O25" s="15">
-        <f xml:space="preserve"> N25*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4734</v>
       </c>
     </row>
@@ -2299,7 +2314,7 @@
       </c>
       <c r="G26" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8083333333333336</v>
+        <v>5.8111111111111109</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>20</v>
@@ -2326,7 +2341,7 @@
         <v>58500</v>
       </c>
       <c r="O26" s="15">
-        <f xml:space="preserve"> N26*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5265</v>
       </c>
     </row>
@@ -2352,7 +2367,7 @@
       </c>
       <c r="G27" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7722222222222221</v>
+        <v>5.7750000000000004</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>72</v>
@@ -2379,7 +2394,7 @@
         <v>46500</v>
       </c>
       <c r="O27" s="15">
-        <f xml:space="preserve"> N27*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4185</v>
       </c>
     </row>
@@ -2405,7 +2420,7 @@
       </c>
       <c r="G28" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.447222222222222</v>
+        <v>5.45</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>72</v>
@@ -2432,7 +2447,7 @@
         <v>56200</v>
       </c>
       <c r="O28" s="15">
-        <f xml:space="preserve"> N28*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5058</v>
       </c>
     </row>
@@ -2458,7 +2473,7 @@
       </c>
       <c r="G29" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1527777777777777</v>
+        <v>5.1555555555555559</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>20</v>
@@ -2485,7 +2500,7 @@
         <v>54900</v>
       </c>
       <c r="O29" s="15">
-        <f xml:space="preserve"> N29*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4941</v>
       </c>
     </row>
@@ -2511,7 +2526,7 @@
       </c>
       <c r="G30" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>5.15</v>
+        <v>5.1527777777777777</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>22</v>
@@ -2538,7 +2553,7 @@
         <v>47900</v>
       </c>
       <c r="O30" s="15">
-        <f xml:space="preserve"> N30*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4311</v>
       </c>
     </row>
@@ -2564,7 +2579,7 @@
       </c>
       <c r="G31" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9000000000000004</v>
+        <v>4.9027777777777777</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>72</v>
@@ -2591,7 +2606,7 @@
         <v>49600</v>
       </c>
       <c r="O31" s="15">
-        <f xml:space="preserve"> N31*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4464</v>
       </c>
     </row>
@@ -2617,7 +2632,7 @@
       </c>
       <c r="G32" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8916666666666666</v>
+        <v>4.8944444444444448</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>72</v>
@@ -2644,7 +2659,7 @@
         <v>35600</v>
       </c>
       <c r="O32" s="15">
-        <f xml:space="preserve"> N32*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>3204</v>
       </c>
     </row>
@@ -2670,7 +2685,7 @@
       </c>
       <c r="G33" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7638888888888893</v>
+        <v>4.7666666666666666</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>80</v>
@@ -2697,7 +2712,7 @@
         <v>58500</v>
       </c>
       <c r="O33" s="15">
-        <f xml:space="preserve"> N33*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>5265</v>
       </c>
     </row>
@@ -2723,7 +2738,7 @@
       </c>
       <c r="G34" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7277777777777779</v>
+        <v>4.7305555555555552</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>72</v>
@@ -2750,7 +2765,7 @@
         <v>51400</v>
       </c>
       <c r="O34" s="15">
-        <f xml:space="preserve"> N34*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>4626</v>
       </c>
     </row>
@@ -2776,7 +2791,7 @@
       </c>
       <c r="G35" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8888888888888888</v>
+        <v>3.8916666666666666</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>22</v>
@@ -2803,7 +2818,7 @@
         <v>38600</v>
       </c>
       <c r="O35" s="15">
-        <f xml:space="preserve"> N35*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>3474</v>
       </c>
     </row>
@@ -2829,7 +2844,7 @@
       </c>
       <c r="G36" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8055555555555554</v>
+        <v>3.8083333333333331</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>72</v>
@@ -2856,7 +2871,7 @@
         <v>40500</v>
       </c>
       <c r="O36" s="15">
-        <f xml:space="preserve"> N36*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>3645</v>
       </c>
     </row>
@@ -2882,7 +2897,7 @@
       </c>
       <c r="G37" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>10.741666666666667</v>
+        <v>10.744444444444444</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>33</v>
@@ -2909,7 +2924,7 @@
         <v>96400</v>
       </c>
       <c r="O37" s="15">
-        <f xml:space="preserve"> N37*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>8676</v>
       </c>
     </row>
@@ -2935,7 +2950,7 @@
       </c>
       <c r="G38" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3833333333333333</v>
+        <v>3.3861111111111111</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>35</v>
@@ -2962,7 +2977,7 @@
         <v>37000</v>
       </c>
       <c r="O38" s="15">
-        <f xml:space="preserve"> N38*pension_rate</f>
+        <f t="shared" si="5"/>
         <v>3330</v>
       </c>
     </row>

</xml_diff>